<commit_message>
Adjust Standing Right Kick animation and frame data, allow simultanous hits
</commit_message>
<xml_diff>
--- a/frameData.xlsx
+++ b/frameData.xlsx
@@ -425,8 +425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -464,6 +464,7 @@
         <v>1</v>
       </c>
       <c r="B3">
+        <f>B23</f>
         <v>8</v>
       </c>
       <c r="C3">
@@ -489,14 +490,15 @@
         <v>2</v>
       </c>
       <c r="B4">
+        <f t="shared" ref="B4:B18" si="0">B24</f>
         <v>12</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C18" si="0">F4+B4-E4+5</f>
+        <f t="shared" ref="C4:C18" si="1">F4+B4-E4+5</f>
         <v>4</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D18" si="1">G4+B4-E4</f>
+        <f t="shared" ref="D4:D18" si="2">G4+B4-E4</f>
         <v>-4</v>
       </c>
       <c r="E4">
@@ -514,14 +516,15 @@
         <v>3</v>
       </c>
       <c r="B5">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="D5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-15</v>
       </c>
       <c r="E5">
@@ -539,24 +542,25 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>14</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="D6">
-        <f t="shared" si="1"/>
+        <f>G6+B6-E6</f>
         <v>-6</v>
       </c>
       <c r="E6">
         <v>40</v>
       </c>
       <c r="F6">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G6">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -564,14 +568,15 @@
         <v>5</v>
       </c>
       <c r="B7">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-3</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-3</v>
       </c>
       <c r="E7">
@@ -589,14 +594,15 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>14</v>
-      </c>
-      <c r="C8">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
       <c r="D8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-8</v>
       </c>
       <c r="E8">
@@ -614,14 +620,15 @@
         <v>7</v>
       </c>
       <c r="B9">
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-25</v>
       </c>
       <c r="E9">
@@ -639,14 +646,15 @@
         <v>8</v>
       </c>
       <c r="B10">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2</v>
       </c>
       <c r="E10">
@@ -664,14 +672,15 @@
         <v>10</v>
       </c>
       <c r="B11">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="D11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="E11">
@@ -689,14 +698,15 @@
         <v>9</v>
       </c>
       <c r="B12">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="D12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-4</v>
       </c>
       <c r="E12">
@@ -714,14 +724,15 @@
         <v>11</v>
       </c>
       <c r="B13">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="D13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-3</v>
       </c>
       <c r="E13">
@@ -739,14 +750,15 @@
         <v>12</v>
       </c>
       <c r="B14">
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-15</v>
       </c>
       <c r="E14">
@@ -764,14 +776,15 @@
         <v>13</v>
       </c>
       <c r="B15">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="D15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-12</v>
       </c>
       <c r="E15">
@@ -789,14 +802,15 @@
         <v>14</v>
       </c>
       <c r="B16">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="D16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E16">
@@ -814,14 +828,15 @@
         <v>15</v>
       </c>
       <c r="B17">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="D17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-15</v>
       </c>
       <c r="E17">
@@ -839,14 +854,15 @@
         <v>16</v>
       </c>
       <c r="B18">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="D18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-10</v>
       </c>
       <c r="E18">
@@ -929,11 +945,11 @@
         <v>40</v>
       </c>
       <c r="F24">
-        <f t="shared" ref="F24:F38" si="2">C24-B24+E24-5</f>
+        <f t="shared" ref="F24:F38" si="3">C24-B24+E24-5</f>
         <v>27</v>
       </c>
       <c r="G24">
-        <f t="shared" ref="G24:G38" si="3">D24-B24+E24</f>
+        <f t="shared" ref="G24:G38" si="4">D24-B24+E24</f>
         <v>24</v>
       </c>
     </row>
@@ -954,11 +970,11 @@
         <v>50</v>
       </c>
       <c r="F25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="G25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
     </row>
@@ -967,7 +983,7 @@
         <v>4</v>
       </c>
       <c r="B26">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C26">
         <v>16</v>
@@ -979,12 +995,12 @@
         <v>40</v>
       </c>
       <c r="F26">
-        <f t="shared" si="2"/>
-        <v>40</v>
+        <f t="shared" si="3"/>
+        <v>37</v>
       </c>
       <c r="G26">
-        <f t="shared" si="3"/>
-        <v>23</v>
+        <f t="shared" si="4"/>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1004,11 +1020,11 @@
         <v>30</v>
       </c>
       <c r="F27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="G27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
     </row>
@@ -1029,11 +1045,11 @@
         <v>45</v>
       </c>
       <c r="F28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="G28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
     </row>
@@ -1054,11 +1070,11 @@
         <v>70</v>
       </c>
       <c r="F29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>55</v>
       </c>
       <c r="G29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
     </row>
@@ -1079,11 +1095,11 @@
         <v>40</v>
       </c>
       <c r="F30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="G30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
     </row>
@@ -1104,11 +1120,11 @@
         <v>25</v>
       </c>
       <c r="F31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
     </row>
@@ -1129,11 +1145,11 @@
         <v>35</v>
       </c>
       <c r="F32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="G32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
     </row>
@@ -1154,11 +1170,11 @@
         <v>30</v>
       </c>
       <c r="F33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="G33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
@@ -1179,11 +1195,11 @@
         <v>50</v>
       </c>
       <c r="F34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="G34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
     </row>
@@ -1204,11 +1220,11 @@
         <v>40</v>
       </c>
       <c r="F35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="G35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
     </row>
@@ -1229,11 +1245,11 @@
         <v>35</v>
       </c>
       <c r="F36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="G36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
     </row>
@@ -1254,11 +1270,11 @@
         <v>50</v>
       </c>
       <c r="F37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="G37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
     </row>
@@ -1279,11 +1295,11 @@
         <v>40</v>
       </c>
       <c r="F38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="G38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adjust character physic material, adjust attackbalance
</commit_message>
<xml_diff>
--- a/frameData.xlsx
+++ b/frameData.xlsx
@@ -425,8 +425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -469,7 +469,7 @@
       </c>
       <c r="C3">
         <f>F3+B3-E3+5</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <f>G3+B3-E3</f>
@@ -479,7 +479,7 @@
         <v>30</v>
       </c>
       <c r="F3">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G3">
         <v>25</v>
@@ -521,20 +521,20 @@
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <f t="shared" si="2"/>
-        <v>-15</v>
+        <v>-14</v>
       </c>
       <c r="E5">
         <v>50</v>
       </c>
       <c r="F5">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G5">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -547,7 +547,7 @@
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D6">
         <f>G6+B6-E6</f>
@@ -557,7 +557,7 @@
         <v>40</v>
       </c>
       <c r="F6">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G6">
         <v>20</v>
@@ -573,7 +573,7 @@
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <f t="shared" si="2"/>
@@ -583,7 +583,7 @@
         <v>30</v>
       </c>
       <c r="F7">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G7">
         <v>17</v>
@@ -961,21 +961,21 @@
         <v>20</v>
       </c>
       <c r="C25">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D25">
-        <v>-15</v>
+        <v>-14</v>
       </c>
       <c r="E25">
         <v>50</v>
       </c>
       <c r="F25">
         <f t="shared" si="3"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G25">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -986,7 +986,7 @@
         <v>14</v>
       </c>
       <c r="C26">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D26">
         <v>-6</v>
@@ -996,7 +996,7 @@
       </c>
       <c r="F26">
         <f t="shared" si="3"/>
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G26">
         <f t="shared" si="4"/>
@@ -1011,7 +1011,7 @@
         <v>10</v>
       </c>
       <c r="C27">
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="D27">
         <v>-3</v>
@@ -1021,7 +1021,7 @@
       </c>
       <c r="F27">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G27">
         <f t="shared" si="4"/>

</xml_diff>

<commit_message>
Adjust move balance, new camera logic, modify combo system, add combo damage scaling
</commit_message>
<xml_diff>
--- a/frameData.xlsx
+++ b/frameData.xlsx
@@ -425,8 +425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -469,7 +469,7 @@
       </c>
       <c r="C3">
         <f>F3+B3-E3+5</f>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <f>G3+B3-E3</f>
@@ -479,7 +479,7 @@
         <v>30</v>
       </c>
       <c r="F3">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G3">
         <v>25</v>
@@ -495,7 +495,7 @@
       </c>
       <c r="C4">
         <f t="shared" ref="C4:C18" si="1">F4+B4-E4+5</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D18" si="2">G4+B4-E4</f>
@@ -505,7 +505,7 @@
         <v>40</v>
       </c>
       <c r="F4">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G4">
         <v>24</v>
@@ -911,7 +911,7 @@
         <v>8</v>
       </c>
       <c r="C23">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D23">
         <v>3</v>
@@ -921,7 +921,7 @@
       </c>
       <c r="F23">
         <f>C23-B23+E23-5</f>
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G23">
         <f>D23-B23+E23</f>
@@ -936,7 +936,7 @@
         <v>12</v>
       </c>
       <c r="C24">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D24">
         <v>-4</v>
@@ -946,7 +946,7 @@
       </c>
       <c r="F24">
         <f t="shared" ref="F24:F38" si="3">C24-B24+E24-5</f>
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G24">
         <f t="shared" ref="G24:G38" si="4">D24-B24+E24</f>
@@ -986,7 +986,7 @@
         <v>14</v>
       </c>
       <c r="C26">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D26">
         <v>-6</v>
@@ -996,7 +996,7 @@
       </c>
       <c r="F26">
         <f t="shared" si="3"/>
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G26">
         <f t="shared" si="4"/>
@@ -1036,7 +1036,7 @@
         <v>14</v>
       </c>
       <c r="C28">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D28">
         <v>-8</v>
@@ -1046,7 +1046,7 @@
       </c>
       <c r="F28">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G28">
         <f t="shared" si="4"/>

</xml_diff>

<commit_message>
Adjust move balance, fix few bugs, create Player prefab, modify MatchManager
</commit_message>
<xml_diff>
--- a/frameData.xlsx
+++ b/frameData.xlsx
@@ -426,7 +426,7 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -479,9 +479,11 @@
         <v>30</v>
       </c>
       <c r="F3">
+        <f>F23</f>
         <v>25</v>
       </c>
       <c r="G3">
+        <f>G23</f>
         <v>25</v>
       </c>
     </row>
@@ -491,7 +493,7 @@
       </c>
       <c r="B4">
         <f t="shared" ref="B4:B18" si="0">B24</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <f t="shared" ref="C4:C18" si="1">F4+B4-E4+5</f>
@@ -505,10 +507,12 @@
         <v>40</v>
       </c>
       <c r="F4">
-        <v>33</v>
+        <f t="shared" ref="F4:G4" si="3">F24</f>
+        <v>35</v>
       </c>
       <c r="G4">
-        <v>24</v>
+        <f t="shared" si="3"/>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -531,9 +535,11 @@
         <v>50</v>
       </c>
       <c r="F5">
+        <f t="shared" ref="F5:G5" si="4">F25</f>
         <v>26</v>
       </c>
       <c r="G5">
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
     </row>
@@ -547,7 +553,7 @@
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6">
         <f>G6+B6-E6</f>
@@ -557,9 +563,11 @@
         <v>40</v>
       </c>
       <c r="F6">
-        <v>33</v>
+        <f t="shared" ref="F6:G6" si="5">F26</f>
+        <v>34</v>
       </c>
       <c r="G6">
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
     </row>
@@ -583,9 +591,11 @@
         <v>30</v>
       </c>
       <c r="F7">
+        <f t="shared" ref="F7:G7" si="6">F27</f>
         <v>18</v>
       </c>
       <c r="G7">
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
     </row>
@@ -599,7 +609,7 @@
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D8">
         <f t="shared" si="2"/>
@@ -609,9 +619,11 @@
         <v>45</v>
       </c>
       <c r="F8">
-        <v>40</v>
+        <f t="shared" ref="F8:G8" si="7">F28</f>
+        <v>41</v>
       </c>
       <c r="G8">
+        <f t="shared" si="7"/>
         <v>23</v>
       </c>
     </row>
@@ -635,9 +647,11 @@
         <v>70</v>
       </c>
       <c r="F9">
+        <f t="shared" ref="F9:G9" si="8">F29</f>
         <v>55</v>
       </c>
       <c r="G9">
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
     </row>
@@ -661,9 +675,11 @@
         <v>40</v>
       </c>
       <c r="F10">
+        <f t="shared" ref="F10:G10" si="9">F30</f>
         <v>28</v>
       </c>
       <c r="G10">
+        <f t="shared" si="9"/>
         <v>28</v>
       </c>
     </row>
@@ -687,9 +703,11 @@
         <v>25</v>
       </c>
       <c r="F11">
+        <f t="shared" ref="F11:G11" si="10">F31</f>
         <v>18</v>
       </c>
       <c r="G11">
+        <f t="shared" si="10"/>
         <v>22</v>
       </c>
     </row>
@@ -713,9 +731,11 @@
         <v>35</v>
       </c>
       <c r="F12">
+        <f t="shared" ref="F12:G12" si="11">F32</f>
         <v>22</v>
       </c>
       <c r="G12">
+        <f t="shared" si="11"/>
         <v>17</v>
       </c>
     </row>
@@ -739,9 +759,11 @@
         <v>30</v>
       </c>
       <c r="F13">
+        <f t="shared" ref="F13:G13" si="12">F33</f>
         <v>12</v>
       </c>
       <c r="G13">
+        <f t="shared" si="12"/>
         <v>12</v>
       </c>
     </row>
@@ -755,7 +777,7 @@
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
@@ -765,9 +787,11 @@
         <v>50</v>
       </c>
       <c r="F14">
-        <v>50</v>
+        <f t="shared" ref="F14:G14" si="13">F34</f>
+        <v>44</v>
       </c>
       <c r="G14">
+        <f t="shared" si="13"/>
         <v>14</v>
       </c>
     </row>
@@ -791,9 +815,11 @@
         <v>40</v>
       </c>
       <c r="F15">
+        <f t="shared" ref="F15:G15" si="14">F35</f>
         <v>40</v>
       </c>
       <c r="G15">
+        <f t="shared" si="14"/>
         <v>10</v>
       </c>
     </row>
@@ -817,9 +843,11 @@
         <v>35</v>
       </c>
       <c r="F16">
+        <f t="shared" ref="F16:G16" si="15">F36</f>
         <v>22</v>
       </c>
       <c r="G16">
+        <f t="shared" si="15"/>
         <v>23</v>
       </c>
     </row>
@@ -833,7 +861,7 @@
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D17">
         <f t="shared" si="2"/>
@@ -843,9 +871,11 @@
         <v>50</v>
       </c>
       <c r="F17">
-        <v>60</v>
+        <f t="shared" ref="F17:G17" si="16">F37</f>
+        <v>50</v>
       </c>
       <c r="G17">
+        <f t="shared" si="16"/>
         <v>10</v>
       </c>
     </row>
@@ -869,9 +899,11 @@
         <v>40</v>
       </c>
       <c r="F18">
+        <f t="shared" ref="F18:G18" si="17">F38</f>
         <v>40</v>
       </c>
       <c r="G18">
+        <f t="shared" si="17"/>
         <v>19</v>
       </c>
     </row>
@@ -933,7 +965,7 @@
         <v>2</v>
       </c>
       <c r="B24">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C24">
         <v>10</v>
@@ -945,12 +977,12 @@
         <v>40</v>
       </c>
       <c r="F24">
-        <f t="shared" ref="F24:F38" si="3">C24-B24+E24-5</f>
-        <v>33</v>
+        <f t="shared" ref="F24:F38" si="18">C24-B24+E24-5</f>
+        <v>35</v>
       </c>
       <c r="G24">
-        <f t="shared" ref="G24:G38" si="4">D24-B24+E24</f>
-        <v>24</v>
+        <f t="shared" ref="G24:G38" si="19">D24-B24+E24</f>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -970,11 +1002,11 @@
         <v>50</v>
       </c>
       <c r="F25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>26</v>
       </c>
       <c r="G25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>16</v>
       </c>
     </row>
@@ -986,7 +1018,7 @@
         <v>14</v>
       </c>
       <c r="C26">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D26">
         <v>-6</v>
@@ -995,11 +1027,11 @@
         <v>40</v>
       </c>
       <c r="F26">
-        <f t="shared" si="3"/>
-        <v>35</v>
+        <f t="shared" si="18"/>
+        <v>34</v>
       </c>
       <c r="G26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>20</v>
       </c>
     </row>
@@ -1020,11 +1052,11 @@
         <v>30</v>
       </c>
       <c r="F27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>18</v>
       </c>
       <c r="G27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>17</v>
       </c>
     </row>
@@ -1045,11 +1077,11 @@
         <v>45</v>
       </c>
       <c r="F28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>41</v>
       </c>
       <c r="G28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>23</v>
       </c>
     </row>
@@ -1070,11 +1102,11 @@
         <v>70</v>
       </c>
       <c r="F29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>55</v>
       </c>
       <c r="G29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>17</v>
       </c>
     </row>
@@ -1095,11 +1127,11 @@
         <v>40</v>
       </c>
       <c r="F30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>28</v>
       </c>
       <c r="G30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>28</v>
       </c>
     </row>
@@ -1120,11 +1152,11 @@
         <v>25</v>
       </c>
       <c r="F31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>18</v>
       </c>
       <c r="G31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>22</v>
       </c>
     </row>
@@ -1145,11 +1177,11 @@
         <v>35</v>
       </c>
       <c r="F32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>22</v>
       </c>
       <c r="G32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>17</v>
       </c>
     </row>
@@ -1170,11 +1202,11 @@
         <v>30</v>
       </c>
       <c r="F33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="G33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>12</v>
       </c>
     </row>
@@ -1186,7 +1218,7 @@
         <v>21</v>
       </c>
       <c r="C34">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D34">
         <v>-15</v>
@@ -1195,11 +1227,11 @@
         <v>50</v>
       </c>
       <c r="F34">
-        <f t="shared" si="3"/>
-        <v>50</v>
+        <f t="shared" si="18"/>
+        <v>44</v>
       </c>
       <c r="G34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>14</v>
       </c>
     </row>
@@ -1220,11 +1252,11 @@
         <v>40</v>
       </c>
       <c r="F35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>40</v>
       </c>
       <c r="G35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>10</v>
       </c>
     </row>
@@ -1245,11 +1277,11 @@
         <v>35</v>
       </c>
       <c r="F36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>22</v>
       </c>
       <c r="G36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>23</v>
       </c>
     </row>
@@ -1261,7 +1293,7 @@
         <v>25</v>
       </c>
       <c r="C37">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D37">
         <v>-15</v>
@@ -1270,11 +1302,11 @@
         <v>50</v>
       </c>
       <c r="F37">
-        <f t="shared" si="3"/>
-        <v>60</v>
+        <f t="shared" si="18"/>
+        <v>50</v>
       </c>
       <c r="G37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>10</v>
       </c>
     </row>
@@ -1295,11 +1327,11 @@
         <v>40</v>
       </c>
       <c r="F38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>40</v>
       </c>
       <c r="G38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modify combo damage scaling and adjust maximum health to compensate for raised combo damage, adjust move balance
</commit_message>
<xml_diff>
--- a/frameData.xlsx
+++ b/frameData.xlsx
@@ -426,7 +426,7 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -529,7 +529,7 @@
       </c>
       <c r="D5">
         <f t="shared" si="2"/>
-        <v>-14</v>
+        <v>-12</v>
       </c>
       <c r="E5">
         <v>50</v>
@@ -540,7 +540,7 @@
       </c>
       <c r="G5">
         <f t="shared" si="4"/>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -996,7 +996,7 @@
         <v>1</v>
       </c>
       <c r="D25">
-        <v>-14</v>
+        <v>-12</v>
       </c>
       <c r="E25">
         <v>50</v>
@@ -1007,7 +1007,7 @@
       </c>
       <c r="G25">
         <f t="shared" si="19"/>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:7">

</xml_diff>

<commit_message>
Adjust move animation and balance
</commit_message>
<xml_diff>
--- a/frameData.xlsx
+++ b/frameData.xlsx
@@ -425,7 +425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -493,11 +493,11 @@
       </c>
       <c r="B4">
         <f t="shared" ref="B4:B18" si="0">B24</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <f t="shared" ref="C4:C18" si="1">F4+B4-E4+5</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D18" si="2">G4+B4-E4</f>
@@ -508,11 +508,11 @@
       </c>
       <c r="F4">
         <f t="shared" ref="F4:G4" si="3">F24</f>
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G4">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -965,10 +965,10 @@
         <v>2</v>
       </c>
       <c r="B24">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C24">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D24">
         <v>-4</v>
@@ -978,11 +978,11 @@
       </c>
       <c r="F24">
         <f t="shared" ref="F24:F38" si="18">C24-B24+E24-5</f>
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G24">
         <f t="shared" ref="G24:G38" si="19">D24-B24+E24</f>
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:7">

</xml_diff>

<commit_message>
Fix some animation issues, make unstanced crouch faster, adjust move balance, adjust animation, start preparing debug round counter for new functions
</commit_message>
<xml_diff>
--- a/frameData.xlsx
+++ b/frameData.xlsx
@@ -432,7 +432,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -473,7 +473,7 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <f>B27</f>
+        <f t="shared" ref="B3:B20" si="0">B27</f>
         <v>8</v>
       </c>
       <c r="C3">
@@ -502,27 +502,27 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <f>B28</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C18" si="0">F4+B4-E4+5</f>
+        <f t="shared" ref="C4:C18" si="1">F4+B4-E4+5</f>
         <v>9</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D18" si="1">G4+B4-E4</f>
+        <f t="shared" ref="D4:D18" si="2">G4+B4-E4</f>
         <v>-4</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E20" si="2">E28</f>
+        <f t="shared" ref="E4:E20" si="3">E28</f>
         <v>40</v>
       </c>
       <c r="F4">
-        <f>F28</f>
+        <f t="shared" ref="F4:G20" si="4">F28</f>
         <v>31</v>
       </c>
       <c r="G4">
-        <f>G28</f>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
     </row>
@@ -531,27 +531,27 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <f>B29</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="D5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-12</v>
       </c>
       <c r="E5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="F5">
-        <f>F29</f>
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
       <c r="G5">
-        <f>G29</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
     </row>
@@ -560,11 +560,11 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <f>B30</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="D6">
@@ -572,15 +572,15 @@
         <v>-6</v>
       </c>
       <c r="E6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="F6">
-        <f>F30</f>
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
       <c r="G6">
-        <f>G30</f>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
     </row>
@@ -589,27 +589,27 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <f>B31</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-3</v>
       </c>
       <c r="E7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="F7">
-        <f>F31</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G7">
-        <f>G31</f>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
     </row>
@@ -618,27 +618,27 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <f>B32</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-8</v>
       </c>
       <c r="E8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="F8">
-        <f>F32</f>
+        <f t="shared" si="4"/>
         <v>41</v>
       </c>
       <c r="G8">
-        <f>G32</f>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
     </row>
@@ -647,27 +647,27 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <f>B33</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-25</v>
       </c>
       <c r="E9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
       <c r="F9">
-        <f>F33</f>
+        <f t="shared" si="4"/>
         <v>55</v>
       </c>
       <c r="G9">
-        <f>G33</f>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
     </row>
@@ -676,27 +676,27 @@
         <v>16</v>
       </c>
       <c r="B10">
-        <f>B34</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2</v>
       </c>
       <c r="E10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="F10">
-        <f>F34</f>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="G10">
-        <f>G34</f>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
     </row>
@@ -705,27 +705,27 @@
         <v>17</v>
       </c>
       <c r="B11">
-        <f>B35</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="D11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="E11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="F11">
-        <f>F35</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G11">
-        <f>G35</f>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
     </row>
@@ -734,27 +734,27 @@
         <v>18</v>
       </c>
       <c r="B12">
-        <f>B36</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="D12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-4</v>
       </c>
       <c r="E12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="F12">
-        <f>F36</f>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="G12">
-        <f>G36</f>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
     </row>
@@ -763,27 +763,27 @@
         <v>19</v>
       </c>
       <c r="B13">
-        <f>B37</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="D13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-3</v>
       </c>
       <c r="E13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="F13">
-        <f>F37</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="G13">
-        <f>G37</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
@@ -792,27 +792,27 @@
         <v>20</v>
       </c>
       <c r="B14">
-        <f>B38</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-15</v>
       </c>
       <c r="E14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="F14">
-        <f>F38</f>
+        <f t="shared" si="4"/>
         <v>44</v>
       </c>
       <c r="G14">
-        <f>G38</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
     </row>
@@ -821,27 +821,27 @@
         <v>21</v>
       </c>
       <c r="B15">
-        <f>B39</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="D15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-12</v>
       </c>
       <c r="E15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="F15">
-        <f>F39</f>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="G15">
-        <f>G39</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
     </row>
@@ -850,27 +850,27 @@
         <v>22</v>
       </c>
       <c r="B16">
-        <f>B40</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="D16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="F16">
-        <f>F40</f>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="G16">
-        <f>G40</f>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
     </row>
@@ -879,27 +879,27 @@
         <v>23</v>
       </c>
       <c r="B17">
-        <f>B41</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="D17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-15</v>
       </c>
       <c r="E17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="F17">
-        <f>F41</f>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="G17">
-        <f>G41</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
     </row>
@@ -908,27 +908,27 @@
         <v>24</v>
       </c>
       <c r="B18">
-        <f>B42</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="D18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-10</v>
       </c>
       <c r="E18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="F18">
-        <f>F42</f>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="G18">
-        <f>G42</f>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
     </row>
@@ -937,28 +937,28 @@
         <v>25</v>
       </c>
       <c r="B19">
-        <f>B43</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="C19">
-        <f t="shared" ref="C19:C20" si="3">F19+B19-E19+5</f>
+        <f t="shared" ref="C19:C20" si="5">F19+B19-E19+5</f>
         <v>30</v>
       </c>
       <c r="D19">
-        <f t="shared" ref="D19:D20" si="4">G19+B19-E19</f>
-        <v>8</v>
+        <f t="shared" ref="D19:D20" si="6">G19+B19-E19</f>
+        <v>6</v>
       </c>
       <c r="E19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="F19">
-        <f>F43</f>
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
       <c r="G19">
-        <f>G43</f>
-        <v>28</v>
+        <f t="shared" si="4"/>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -966,27 +966,27 @@
         <v>26</v>
       </c>
       <c r="B20">
-        <f>B44</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="C20">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E20">
         <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="F20">
-        <f>F44</f>
+        <f t="shared" si="4"/>
         <v>36</v>
       </c>
       <c r="G20">
-        <f>G44</f>
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
     </row>
@@ -1060,11 +1060,11 @@
         <v>40</v>
       </c>
       <c r="F28">
-        <f t="shared" ref="F28:F44" si="5">C28-B28+E28-5</f>
+        <f t="shared" ref="F28:F44" si="7">C28-B28+E28-5</f>
         <v>31</v>
       </c>
       <c r="G28">
-        <f t="shared" ref="G28:G44" si="6">D28-B28+E28</f>
+        <f t="shared" ref="G28:G44" si="8">D28-B28+E28</f>
         <v>23</v>
       </c>
     </row>
@@ -1085,11 +1085,11 @@
         <v>50</v>
       </c>
       <c r="F29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>26</v>
       </c>
       <c r="G29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
     </row>
@@ -1110,11 +1110,11 @@
         <v>40</v>
       </c>
       <c r="F30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>35</v>
       </c>
       <c r="G30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
     </row>
@@ -1135,11 +1135,11 @@
         <v>30</v>
       </c>
       <c r="F31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>18</v>
       </c>
       <c r="G31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
     </row>
@@ -1160,11 +1160,11 @@
         <v>45</v>
       </c>
       <c r="F32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>41</v>
       </c>
       <c r="G32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>23</v>
       </c>
     </row>
@@ -1185,11 +1185,11 @@
         <v>70</v>
       </c>
       <c r="F33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>55</v>
       </c>
       <c r="G33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
     </row>
@@ -1210,11 +1210,11 @@
         <v>40</v>
       </c>
       <c r="F34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>28</v>
       </c>
       <c r="G34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>28</v>
       </c>
     </row>
@@ -1235,11 +1235,11 @@
         <v>25</v>
       </c>
       <c r="F35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>18</v>
       </c>
       <c r="G35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>22</v>
       </c>
     </row>
@@ -1260,11 +1260,11 @@
         <v>35</v>
       </c>
       <c r="F36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>22</v>
       </c>
       <c r="G36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
     </row>
@@ -1285,11 +1285,11 @@
         <v>30</v>
       </c>
       <c r="F37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
       <c r="G37">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
     </row>
@@ -1310,11 +1310,11 @@
         <v>50</v>
       </c>
       <c r="F38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44</v>
       </c>
       <c r="G38">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>14</v>
       </c>
     </row>
@@ -1335,11 +1335,11 @@
         <v>40</v>
       </c>
       <c r="F39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>40</v>
       </c>
       <c r="G39">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
     </row>
@@ -1360,11 +1360,11 @@
         <v>35</v>
       </c>
       <c r="F40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>22</v>
       </c>
       <c r="G40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>23</v>
       </c>
     </row>
@@ -1385,11 +1385,11 @@
         <v>50</v>
       </c>
       <c r="F41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>50</v>
       </c>
       <c r="G41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
     </row>
@@ -1410,11 +1410,11 @@
         <v>40</v>
       </c>
       <c r="F42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>40</v>
       </c>
       <c r="G42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
     </row>
@@ -1429,18 +1429,18 @@
         <v>30</v>
       </c>
       <c r="D43">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E43">
         <v>45</v>
       </c>
       <c r="F43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>45</v>
       </c>
       <c r="G43">
-        <f t="shared" si="6"/>
-        <v>28</v>
+        <f t="shared" si="8"/>
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1460,11 +1460,11 @@
         <v>45</v>
       </c>
       <c r="F44">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>36</v>
       </c>
       <c r="G44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adjust animation, adjust move balance
</commit_message>
<xml_diff>
--- a/frameData.xlsx
+++ b/frameData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
   <si>
     <t>name</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Backdashing Left Kick</t>
+  </si>
+  <si>
+    <t>Running Right Punch</t>
   </si>
 </sst>
 </file>
@@ -429,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -473,7 +476,7 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B20" si="0">B27</f>
+        <f t="shared" ref="B3:B21" si="0">B27</f>
         <v>8</v>
       </c>
       <c r="C3">
@@ -514,11 +517,11 @@
         <v>-4</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E20" si="3">E28</f>
+        <f t="shared" ref="E4:E21" si="3">E28</f>
         <v>40</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:G20" si="4">F28</f>
+        <f t="shared" ref="F4:G21" si="4">F28</f>
         <v>31</v>
       </c>
       <c r="G4">
@@ -990,6 +993,35 @@
         <v>21</v>
       </c>
     </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ref="C21" si="7">F21+B21-E21+5</f>
+        <v>21</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ref="D21" si="8">G21+B21-E21</f>
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="3"/>
+        <v>55</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="4"/>
+        <v>38</v>
+      </c>
+    </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>7</v>
@@ -1060,11 +1092,11 @@
         <v>40</v>
       </c>
       <c r="F28">
-        <f t="shared" ref="F28:F44" si="7">C28-B28+E28-5</f>
+        <f t="shared" ref="F28:F45" si="9">C28-B28+E28-5</f>
         <v>31</v>
       </c>
       <c r="G28">
-        <f t="shared" ref="G28:G44" si="8">D28-B28+E28</f>
+        <f t="shared" ref="G28:G45" si="10">D28-B28+E28</f>
         <v>23</v>
       </c>
     </row>
@@ -1085,11 +1117,11 @@
         <v>50</v>
       </c>
       <c r="F29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>26</v>
       </c>
       <c r="G29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>18</v>
       </c>
     </row>
@@ -1110,11 +1142,11 @@
         <v>40</v>
       </c>
       <c r="F30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>35</v>
       </c>
       <c r="G30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>20</v>
       </c>
     </row>
@@ -1135,11 +1167,11 @@
         <v>30</v>
       </c>
       <c r="F31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>18</v>
       </c>
       <c r="G31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>17</v>
       </c>
     </row>
@@ -1160,11 +1192,11 @@
         <v>45</v>
       </c>
       <c r="F32">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>41</v>
       </c>
       <c r="G32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>23</v>
       </c>
     </row>
@@ -1185,11 +1217,11 @@
         <v>70</v>
       </c>
       <c r="F33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>55</v>
       </c>
       <c r="G33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>17</v>
       </c>
     </row>
@@ -1210,11 +1242,11 @@
         <v>40</v>
       </c>
       <c r="F34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>28</v>
       </c>
       <c r="G34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>28</v>
       </c>
     </row>
@@ -1235,11 +1267,11 @@
         <v>25</v>
       </c>
       <c r="F35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>18</v>
       </c>
       <c r="G35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>22</v>
       </c>
     </row>
@@ -1260,11 +1292,11 @@
         <v>35</v>
       </c>
       <c r="F36">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>22</v>
       </c>
       <c r="G36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>17</v>
       </c>
     </row>
@@ -1285,11 +1317,11 @@
         <v>30</v>
       </c>
       <c r="F37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="G37">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
     </row>
@@ -1310,11 +1342,11 @@
         <v>50</v>
       </c>
       <c r="F38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>44</v>
       </c>
       <c r="G38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>14</v>
       </c>
     </row>
@@ -1335,11 +1367,11 @@
         <v>40</v>
       </c>
       <c r="F39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>40</v>
       </c>
       <c r="G39">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
     </row>
@@ -1360,11 +1392,11 @@
         <v>35</v>
       </c>
       <c r="F40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>22</v>
       </c>
       <c r="G40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>23</v>
       </c>
     </row>
@@ -1385,11 +1417,11 @@
         <v>50</v>
       </c>
       <c r="F41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>50</v>
       </c>
       <c r="G41">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
     </row>
@@ -1410,11 +1442,11 @@
         <v>40</v>
       </c>
       <c r="F42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>40</v>
       </c>
       <c r="G42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>19</v>
       </c>
     </row>
@@ -1435,11 +1467,11 @@
         <v>45</v>
       </c>
       <c r="F43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>45</v>
       </c>
       <c r="G43">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>26</v>
       </c>
     </row>
@@ -1460,12 +1492,37 @@
         <v>45</v>
       </c>
       <c r="F44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>36</v>
       </c>
       <c r="G44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" t="s">
+        <v>27</v>
+      </c>
+      <c r="B45">
+        <v>21</v>
+      </c>
+      <c r="C45">
+        <v>21</v>
+      </c>
+      <c r="D45">
+        <v>4</v>
+      </c>
+      <c r="E45">
+        <v>55</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="9"/>
+        <v>50</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="10"/>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add hitspark emission, add blockspark and blockspark emission, lower lighting intensity, change stage colors. adjust move balance
</commit_message>
<xml_diff>
--- a/frameData.xlsx
+++ b/frameData.xlsx
@@ -435,7 +435,7 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -680,7 +680,7 @@
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
@@ -696,11 +696,11 @@
       </c>
       <c r="F10">
         <f t="shared" si="4"/>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G10">
         <f t="shared" si="4"/>
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1230,7 +1230,7 @@
         <v>16</v>
       </c>
       <c r="B34">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C34">
         <v>3</v>
@@ -1243,11 +1243,11 @@
       </c>
       <c r="F34">
         <f t="shared" si="9"/>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G34">
         <f t="shared" si="10"/>
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:7">

</xml_diff>

<commit_message>
Adjust move animation and balance, adjust blockspark spawn position
</commit_message>
<xml_diff>
--- a/frameData.xlsx
+++ b/frameData.xlsx
@@ -435,7 +435,7 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -709,7 +709,7 @@
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
@@ -721,15 +721,15 @@
       </c>
       <c r="E11">
         <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="4"/>
         <v>25</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="4"/>
-        <v>18</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="4"/>
-        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -974,7 +974,7 @@
       </c>
       <c r="C20">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D20">
         <f t="shared" si="6"/>
@@ -986,7 +986,7 @@
       </c>
       <c r="F20">
         <f t="shared" si="4"/>
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G20">
         <f t="shared" si="4"/>
@@ -1255,7 +1255,7 @@
         <v>17</v>
       </c>
       <c r="B35">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C35">
         <v>9</v>
@@ -1264,15 +1264,15 @@
         <v>8</v>
       </c>
       <c r="E35">
+        <v>30</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="9"/>
+        <v>21</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="10"/>
         <v>25</v>
-      </c>
-      <c r="F35">
-        <f t="shared" si="9"/>
-        <v>18</v>
-      </c>
-      <c r="G35">
-        <f t="shared" si="10"/>
-        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1483,7 +1483,7 @@
         <v>24</v>
       </c>
       <c r="C44">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -1493,7 +1493,7 @@
       </c>
       <c r="F44">
         <f t="shared" si="9"/>
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G44">
         <f t="shared" si="10"/>

</xml_diff>

<commit_message>
Adjust animation, adjust move balance, slow down some attack animations on block
</commit_message>
<xml_diff>
--- a/frameData.xlsx
+++ b/frameData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
   <si>
     <t>name</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Running Right Punch</t>
+  </si>
+  <si>
+    <t>artificial blockstun lengthening</t>
   </si>
 </sst>
 </file>
@@ -116,12 +119,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -136,8 +145,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -432,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -738,7 +749,7 @@
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
@@ -754,11 +765,11 @@
       </c>
       <c r="F12">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G12">
         <f t="shared" si="4"/>
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -767,15 +778,15 @@
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D13">
         <f t="shared" si="2"/>
-        <v>-3</v>
+        <v>7</v>
       </c>
       <c r="E13">
         <f t="shared" si="3"/>
@@ -783,11 +794,11 @@
       </c>
       <c r="F13">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G13">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -804,7 +815,7 @@
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
-        <v>-15</v>
+        <v>-7</v>
       </c>
       <c r="E14">
         <f t="shared" si="3"/>
@@ -816,7 +827,7 @@
       </c>
       <c r="G14">
         <f t="shared" si="4"/>
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -833,7 +844,7 @@
       </c>
       <c r="D15">
         <f t="shared" si="2"/>
-        <v>-12</v>
+        <v>-2</v>
       </c>
       <c r="E15">
         <f t="shared" si="3"/>
@@ -845,7 +856,7 @@
       </c>
       <c r="G15">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -891,7 +902,7 @@
       </c>
       <c r="D17">
         <f t="shared" si="2"/>
-        <v>-15</v>
+        <v>-5</v>
       </c>
       <c r="E17">
         <f t="shared" si="3"/>
@@ -903,7 +914,7 @@
       </c>
       <c r="G17">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -978,7 +989,7 @@
       </c>
       <c r="D20">
         <f t="shared" si="6"/>
-        <v>-8</v>
+        <v>5</v>
       </c>
       <c r="E20">
         <f t="shared" si="3"/>
@@ -990,7 +1001,7 @@
       </c>
       <c r="G20">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1096,7 +1107,7 @@
         <v>31</v>
       </c>
       <c r="G28">
-        <f t="shared" ref="G28:G45" si="10">D28-B28+E28</f>
+        <f>D28-B28+E28</f>
         <v>23</v>
       </c>
     </row>
@@ -1121,7 +1132,7 @@
         <v>26</v>
       </c>
       <c r="G29">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="G28:G45" si="10">D29-B29+E29</f>
         <v>18</v>
       </c>
     </row>
@@ -1280,7 +1291,7 @@
         <v>18</v>
       </c>
       <c r="B36">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C36">
         <v>6</v>
@@ -1293,11 +1304,11 @@
       </c>
       <c r="F36">
         <f t="shared" si="9"/>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G36">
         <f t="shared" si="10"/>
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1305,10 +1316,10 @@
         <v>19</v>
       </c>
       <c r="B37">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C37">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D37">
         <v>-3</v>
@@ -1318,11 +1329,11 @@
       </c>
       <c r="F37">
         <f t="shared" si="9"/>
-        <v>12</v>
-      </c>
-      <c r="G37">
-        <f t="shared" si="10"/>
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="G37" s="1">
+        <f>(D37-B37+E37)*2</f>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1336,7 +1347,7 @@
         <v>20</v>
       </c>
       <c r="D38">
-        <v>-15</v>
+        <v>-18</v>
       </c>
       <c r="E38">
         <v>50</v>
@@ -1345,9 +1356,9 @@
         <f t="shared" si="9"/>
         <v>44</v>
       </c>
-      <c r="G38">
-        <f t="shared" si="10"/>
-        <v>14</v>
+      <c r="G38" s="1">
+        <f>(D38-B38+E38)*2</f>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1370,9 +1381,9 @@
         <f t="shared" si="9"/>
         <v>40</v>
       </c>
-      <c r="G39">
-        <f t="shared" si="10"/>
-        <v>10</v>
+      <c r="G39" s="1">
+        <f>(D39-B39+E39)*2</f>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1420,9 +1431,9 @@
         <f t="shared" si="9"/>
         <v>50</v>
       </c>
-      <c r="G41">
-        <f t="shared" si="10"/>
-        <v>10</v>
+      <c r="G41" s="1">
+        <f>(D41-B41+E41)*2</f>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1495,9 +1506,9 @@
         <f t="shared" si="9"/>
         <v>39</v>
       </c>
-      <c r="G44">
-        <f t="shared" si="10"/>
-        <v>13</v>
+      <c r="G44" s="1">
+        <f>(D44-B44+E44)*2</f>
+        <v>26</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1523,6 +1534,12 @@
       <c r="G45">
         <f t="shared" si="10"/>
         <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="1"/>
+      <c r="B47" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add running left kick
</commit_message>
<xml_diff>
--- a/frameData.xlsx
+++ b/frameData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="30">
   <si>
     <t>name</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>artificial blockstun lengthening</t>
+  </si>
+  <si>
+    <t>RunningLeftKick</t>
   </si>
 </sst>
 </file>
@@ -445,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -487,7 +490,7 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B21" si="0">B27</f>
+        <f t="shared" ref="B3:B22" si="0">B27</f>
         <v>8</v>
       </c>
       <c r="C3">
@@ -528,11 +531,11 @@
         <v>-4</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E21" si="3">E28</f>
+        <f t="shared" ref="E4:E22" si="3">E28</f>
         <v>40</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:G21" si="4">F28</f>
+        <f t="shared" ref="F4:G22" si="4">F28</f>
         <v>31</v>
       </c>
       <c r="G4">
@@ -1033,6 +1036,35 @@
         <v>38</v>
       </c>
     </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C22">
+        <f t="shared" ref="C22" si="9">F22+B22-E22+5</f>
+        <v>15</v>
+      </c>
+      <c r="D22">
+        <f t="shared" ref="D22" si="10">G22+B22-E22</f>
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="3"/>
+        <v>65</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+    </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>7</v>
@@ -1103,7 +1135,7 @@
         <v>40</v>
       </c>
       <c r="F28">
-        <f t="shared" ref="F28:F45" si="9">C28-B28+E28-5</f>
+        <f t="shared" ref="F28:F45" si="11">C28-B28+E28-5</f>
         <v>31</v>
       </c>
       <c r="G28">
@@ -1128,11 +1160,11 @@
         <v>50</v>
       </c>
       <c r="F29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>26</v>
       </c>
       <c r="G29">
-        <f t="shared" ref="G28:G45" si="10">D29-B29+E29</f>
+        <f t="shared" ref="G29:G45" si="12">D29-B29+E29</f>
         <v>18</v>
       </c>
     </row>
@@ -1153,11 +1185,11 @@
         <v>40</v>
       </c>
       <c r="F30">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>35</v>
       </c>
       <c r="G30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>20</v>
       </c>
     </row>
@@ -1178,11 +1210,11 @@
         <v>30</v>
       </c>
       <c r="F31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>18</v>
       </c>
       <c r="G31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>17</v>
       </c>
     </row>
@@ -1203,11 +1235,11 @@
         <v>45</v>
       </c>
       <c r="F32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>42</v>
       </c>
       <c r="G32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>23</v>
       </c>
     </row>
@@ -1228,11 +1260,11 @@
         <v>70</v>
       </c>
       <c r="F33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>55</v>
       </c>
       <c r="G33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>17</v>
       </c>
     </row>
@@ -1253,11 +1285,11 @@
         <v>40</v>
       </c>
       <c r="F34">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>26</v>
       </c>
       <c r="G34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>26</v>
       </c>
     </row>
@@ -1278,11 +1310,11 @@
         <v>30</v>
       </c>
       <c r="F35">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>21</v>
       </c>
       <c r="G35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>25</v>
       </c>
     </row>
@@ -1303,11 +1335,11 @@
         <v>35</v>
       </c>
       <c r="F36">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>21</v>
       </c>
       <c r="G36">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>16</v>
       </c>
     </row>
@@ -1328,7 +1360,7 @@
         <v>30</v>
       </c>
       <c r="F37">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>13</v>
       </c>
       <c r="G37" s="1">
@@ -1353,7 +1385,7 @@
         <v>50</v>
       </c>
       <c r="F38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>44</v>
       </c>
       <c r="G38" s="1">
@@ -1378,7 +1410,7 @@
         <v>40</v>
       </c>
       <c r="F39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>40</v>
       </c>
       <c r="G39" s="1">
@@ -1403,11 +1435,11 @@
         <v>35</v>
       </c>
       <c r="F40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>22</v>
       </c>
       <c r="G40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>23</v>
       </c>
     </row>
@@ -1428,7 +1460,7 @@
         <v>50</v>
       </c>
       <c r="F41">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>50</v>
       </c>
       <c r="G41" s="1">
@@ -1453,11 +1485,11 @@
         <v>40</v>
       </c>
       <c r="F42">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>40</v>
       </c>
       <c r="G42">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>19</v>
       </c>
     </row>
@@ -1478,11 +1510,11 @@
         <v>45</v>
       </c>
       <c r="F43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>45</v>
       </c>
       <c r="G43">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>26</v>
       </c>
     </row>
@@ -1503,7 +1535,7 @@
         <v>45</v>
       </c>
       <c r="F44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>39</v>
       </c>
       <c r="G44" s="1">
@@ -1528,12 +1560,37 @@
         <v>55</v>
       </c>
       <c r="F45">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>50</v>
       </c>
       <c r="G45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" t="s">
+        <v>29</v>
+      </c>
+      <c r="B46">
+        <v>25</v>
+      </c>
+      <c r="C46">
+        <v>15</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>65</v>
+      </c>
+      <c r="F46">
+        <f t="shared" ref="F46" si="13">C46-B46+E46-5</f>
+        <v>50</v>
+      </c>
+      <c r="G46">
+        <f t="shared" ref="G46" si="14">D46-B46+E46</f>
+        <v>40</v>
       </c>
     </row>
     <row r="47" spans="1:7">

</xml_diff>

<commit_message>
Adjust move balance, add time limit option to settings
</commit_message>
<xml_diff>
--- a/frameData.xlsx
+++ b/frameData.xlsx
@@ -449,7 +449,7 @@
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -843,7 +843,7 @@
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D15">
         <f t="shared" si="2"/>
@@ -855,7 +855,7 @@
       </c>
       <c r="F15">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="G15">
         <f t="shared" si="4"/>
@@ -1401,7 +1401,7 @@
         <v>18</v>
       </c>
       <c r="C39">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D39">
         <v>-12</v>
@@ -1411,7 +1411,7 @@
       </c>
       <c r="F39">
         <f t="shared" si="11"/>
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="G39" s="1">
         <f>(D39-B39+E39)*2</f>

</xml_diff>

<commit_message>
Add running right kick
</commit_message>
<xml_diff>
--- a/frameData.xlsx
+++ b/frameData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>name</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>RunningLeftKick</t>
+  </si>
+  <si>
+    <t>Running Right Kick</t>
   </si>
 </sst>
 </file>
@@ -446,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -486,11 +489,12 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>9</v>
+      <c r="A3" t="str">
+        <f>A27</f>
+        <v>Standing Left Punch</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B22" si="0">B27</f>
+        <f t="shared" ref="B3:B23" si="0">B27</f>
         <v>8</v>
       </c>
       <c r="C3">
@@ -515,73 +519,76 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>10</v>
+      <c r="A4" t="str">
+        <f t="shared" ref="A4:A23" si="1">A28</f>
+        <v>Standing Right Punch</v>
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C18" si="1">F4+B4-E4+5</f>
+        <f t="shared" ref="C4:C18" si="2">F4+B4-E4+5</f>
         <v>9</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D18" si="2">G4+B4-E4</f>
+        <f t="shared" ref="D4:D18" si="3">G4+B4-E4</f>
         <v>-4</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E22" si="3">E28</f>
+        <f t="shared" ref="E4:E23" si="4">E28</f>
         <v>40</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:G22" si="4">F28</f>
+        <f t="shared" ref="F4:G23" si="5">F28</f>
         <v>31</v>
       </c>
       <c r="G4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>11</v>
+      <c r="A5" t="str">
+        <f t="shared" si="1"/>
+        <v>Standing Left Kick</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="C5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="D5">
+        <f t="shared" si="3"/>
+        <v>-12</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="5"/>
+        <v>26</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="str">
+        <f t="shared" si="1"/>
+        <v>Standing Right Kick</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C6">
         <f t="shared" si="2"/>
-        <v>-12</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="3"/>
-        <v>50</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="4"/>
-        <v>26</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="4"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="D6">
@@ -589,479 +596,525 @@
         <v>-6</v>
       </c>
       <c r="E6">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="5"/>
+        <v>35</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="str">
+        <f t="shared" si="1"/>
+        <v>Crouching Left Punch</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="D7">
         <f t="shared" si="3"/>
+        <v>-3</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="str">
+        <f t="shared" si="1"/>
+        <v>Crouching Right Punch</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="3"/>
+        <v>-8</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="5"/>
+        <v>42</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="5"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="str">
+        <f t="shared" si="1"/>
+        <v>Crouching Left Kick</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="3"/>
+        <v>-25</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="4"/>
+        <v>70</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="5"/>
+        <v>55</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="str">
+        <f t="shared" si="1"/>
+        <v>Crouching Right Kick</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
-      <c r="F6">
+      <c r="F10">
+        <f t="shared" si="5"/>
+        <v>26</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="5"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="str">
+        <f t="shared" si="1"/>
+        <v>Dashing Left Punch</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="str">
+        <f t="shared" si="1"/>
+        <v>Dashing Right Punch</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="3"/>
+        <v>-4</v>
+      </c>
+      <c r="E12">
         <f t="shared" si="4"/>
         <v>35</v>
       </c>
-      <c r="G6">
-        <f t="shared" si="4"/>
+      <c r="F12">
+        <f t="shared" si="5"/>
+        <v>27</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="str">
+        <f t="shared" si="1"/>
+        <v>Dashing Left Kick</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="D7">
+    <row r="14" spans="1:7">
+      <c r="A14" t="str">
+        <f t="shared" si="1"/>
+        <v>Dashing Right Kick</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="C14">
         <f t="shared" si="2"/>
-        <v>-3</v>
-      </c>
-      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="D14">
         <f t="shared" si="3"/>
+        <v>-7</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="5"/>
+        <v>44</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="str">
+        <f t="shared" si="1"/>
+        <v>Jumping Left Punch</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="5"/>
+        <v>33</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="str">
+        <f t="shared" si="1"/>
+        <v>Jumping Right Punch</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="4"/>
+        <v>35</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="5"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="str">
+        <f t="shared" si="1"/>
+        <v>Jumping Left Kick</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="F7">
-        <f t="shared" si="4"/>
-        <v>18</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="4"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="1"/>
+      <c r="D17">
+        <f t="shared" si="3"/>
+        <v>-5</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="str">
+        <f t="shared" si="1"/>
+        <v>Jumping Right Kick</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="D8">
-        <f t="shared" si="2"/>
-        <v>-8</v>
-      </c>
-      <c r="E8">
+      <c r="D18">
         <f t="shared" si="3"/>
+        <v>-10</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="str">
+        <f t="shared" si="1"/>
+        <v>Backdashing Left Punch</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C19">
+        <f t="shared" ref="C19:C20" si="6">F19+B19-E19+5</f>
+        <v>30</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ref="D19:D20" si="7">G19+B19-E19</f>
+        <v>6</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
-      <c r="F8">
-        <f t="shared" si="4"/>
-        <v>42</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="4"/>
+      <c r="F19">
+        <f t="shared" si="5"/>
+        <v>45</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="5"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="str">
+        <f t="shared" si="1"/>
+        <v>Backdashing Left Kick</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="6"/>
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
+      <c r="D20">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="5"/>
+        <v>39</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="5"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="str">
+        <f t="shared" si="1"/>
+        <v>Running Right Punch</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ref="C21" si="8">F21+B21-E21+5</f>
+        <v>21</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ref="D21" si="9">G21+B21-E21</f>
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="4"/>
+        <v>55</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="5"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="str">
+        <f t="shared" si="1"/>
+        <v>RunningLeftKick</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C22">
+        <f t="shared" ref="C22" si="10">F22+B22-E22+5</f>
         <v>15</v>
       </c>
-      <c r="B9">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="2"/>
-        <v>-25</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="3"/>
-        <v>70</v>
-      </c>
-      <c r="F9">
+      <c r="D22">
+        <f t="shared" ref="D22" si="11">G22+B22-E22</f>
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="4"/>
+        <v>65</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="str">
+        <f t="shared" si="1"/>
+        <v>Running Right Kick</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ref="C23" si="12">F23+B23-E23+5</f>
+        <v>20</v>
+      </c>
+      <c r="D23">
+        <f t="shared" ref="D23" si="13">G23+B23-E23</f>
+        <v>4</v>
+      </c>
+      <c r="E23">
         <f t="shared" si="4"/>
         <v>55</v>
       </c>
-      <c r="G9">
-        <f t="shared" si="4"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="2"/>
-        <v>-2</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="3"/>
-        <v>40</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="4"/>
-        <v>26</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="4"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="3"/>
-        <v>30</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="4"/>
-        <v>21</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="4"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="2"/>
-        <v>-4</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="3"/>
-        <v>35</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="4"/>
-        <v>27</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="3"/>
-        <v>30</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="4"/>
-        <v>13</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="4"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="2"/>
-        <v>-7</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="3"/>
-        <v>50</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="4"/>
-        <v>44</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="4"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="2"/>
-        <v>-2</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="3"/>
-        <v>40</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="4"/>
-        <v>33</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="4"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="3"/>
-        <v>35</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="4"/>
-        <v>22</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="4"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="2"/>
-        <v>-5</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="3"/>
-        <v>50</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="4"/>
-        <v>50</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="4"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="C18">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="2"/>
-        <v>-10</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="3"/>
-        <v>40</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="4"/>
-        <v>40</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="4"/>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="C19">
-        <f t="shared" ref="C19:C20" si="5">F19+B19-E19+5</f>
-        <v>30</v>
-      </c>
-      <c r="D19">
-        <f t="shared" ref="D19:D20" si="6">G19+B19-E19</f>
-        <v>6</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="3"/>
-        <v>45</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="4"/>
-        <v>45</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="4"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="5"/>
-        <v>23</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="3"/>
-        <v>45</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="4"/>
-        <v>39</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="4"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="C21">
-        <f t="shared" ref="C21" si="7">F21+B21-E21+5</f>
-        <v>21</v>
-      </c>
-      <c r="D21">
-        <f t="shared" ref="D21" si="8">G21+B21-E21</f>
-        <v>4</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="3"/>
-        <v>55</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="4"/>
-        <v>50</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="4"/>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="C22">
-        <f t="shared" ref="C22" si="9">F22+B22-E22+5</f>
-        <v>15</v>
-      </c>
-      <c r="D22">
-        <f t="shared" ref="D22" si="10">G22+B22-E22</f>
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="3"/>
-        <v>65</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="4"/>
-        <v>50</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="4"/>
+      <c r="F23">
+        <f t="shared" si="5"/>
+        <v>51</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="5"/>
         <v>40</v>
       </c>
     </row>
@@ -1135,7 +1188,7 @@
         <v>40</v>
       </c>
       <c r="F28">
-        <f t="shared" ref="F28:F45" si="11">C28-B28+E28-5</f>
+        <f t="shared" ref="F28:F45" si="14">C28-B28+E28-5</f>
         <v>31</v>
       </c>
       <c r="G28">
@@ -1160,11 +1213,11 @@
         <v>50</v>
       </c>
       <c r="F29">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>26</v>
       </c>
       <c r="G29">
-        <f t="shared" ref="G29:G45" si="12">D29-B29+E29</f>
+        <f t="shared" ref="G29:G45" si="15">D29-B29+E29</f>
         <v>18</v>
       </c>
     </row>
@@ -1185,11 +1238,11 @@
         <v>40</v>
       </c>
       <c r="F30">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>35</v>
       </c>
       <c r="G30">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>20</v>
       </c>
     </row>
@@ -1210,11 +1263,11 @@
         <v>30</v>
       </c>
       <c r="F31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>18</v>
       </c>
       <c r="G31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>17</v>
       </c>
     </row>
@@ -1235,11 +1288,11 @@
         <v>45</v>
       </c>
       <c r="F32">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>42</v>
       </c>
       <c r="G32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>23</v>
       </c>
     </row>
@@ -1260,11 +1313,11 @@
         <v>70</v>
       </c>
       <c r="F33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>55</v>
       </c>
       <c r="G33">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>17</v>
       </c>
     </row>
@@ -1285,11 +1338,11 @@
         <v>40</v>
       </c>
       <c r="F34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>26</v>
       </c>
       <c r="G34">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>26</v>
       </c>
     </row>
@@ -1310,11 +1363,11 @@
         <v>30</v>
       </c>
       <c r="F35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>21</v>
       </c>
       <c r="G35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>25</v>
       </c>
     </row>
@@ -1335,11 +1388,11 @@
         <v>35</v>
       </c>
       <c r="F36">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>27</v>
       </c>
       <c r="G36">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>16</v>
       </c>
     </row>
@@ -1360,7 +1413,7 @@
         <v>30</v>
       </c>
       <c r="F37">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>13</v>
       </c>
       <c r="G37" s="1">
@@ -1385,7 +1438,7 @@
         <v>50</v>
       </c>
       <c r="F38">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>44</v>
       </c>
       <c r="G38" s="1">
@@ -1410,7 +1463,7 @@
         <v>40</v>
       </c>
       <c r="F39">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>33</v>
       </c>
       <c r="G39" s="1">
@@ -1435,11 +1488,11 @@
         <v>35</v>
       </c>
       <c r="F40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>22</v>
       </c>
       <c r="G40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>23</v>
       </c>
     </row>
@@ -1460,7 +1513,7 @@
         <v>50</v>
       </c>
       <c r="F41">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>50</v>
       </c>
       <c r="G41" s="1">
@@ -1485,11 +1538,11 @@
         <v>40</v>
       </c>
       <c r="F42">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>40</v>
       </c>
       <c r="G42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>19</v>
       </c>
     </row>
@@ -1510,11 +1563,11 @@
         <v>45</v>
       </c>
       <c r="F43">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>45</v>
       </c>
       <c r="G43">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>26</v>
       </c>
     </row>
@@ -1535,7 +1588,7 @@
         <v>45</v>
       </c>
       <c r="F44">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>39</v>
       </c>
       <c r="G44" s="1">
@@ -1560,11 +1613,11 @@
         <v>55</v>
       </c>
       <c r="F45">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>50</v>
       </c>
       <c r="G45">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>38</v>
       </c>
     </row>
@@ -1585,17 +1638,42 @@
         <v>65</v>
       </c>
       <c r="F46">
-        <f t="shared" ref="F46" si="13">C46-B46+E46-5</f>
+        <f t="shared" ref="F46:F47" si="16">C46-B46+E46-5</f>
         <v>50</v>
       </c>
       <c r="G46">
-        <f t="shared" ref="G46" si="14">D46-B46+E46</f>
+        <f t="shared" ref="G46:G47" si="17">D46-B46+E46</f>
         <v>40</v>
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="1"/>
-      <c r="B47" s="2" t="s">
+      <c r="A47" t="s">
+        <v>30</v>
+      </c>
+      <c r="B47">
+        <v>19</v>
+      </c>
+      <c r="C47">
+        <v>20</v>
+      </c>
+      <c r="D47">
+        <v>4</v>
+      </c>
+      <c r="E47">
+        <v>55</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="16"/>
+        <v>51</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="17"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="1"/>
+      <c r="B48" s="2" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adjust animation and move balance
</commit_message>
<xml_diff>
--- a/frameData.xlsx
+++ b/frameData.xlsx
@@ -452,7 +452,7 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -795,7 +795,7 @@
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13">
         <f t="shared" si="2"/>
@@ -803,7 +803,7 @@
       </c>
       <c r="D13">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E13">
         <f t="shared" si="4"/>
@@ -811,11 +811,11 @@
       </c>
       <c r="F13">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G13">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1401,7 +1401,7 @@
         <v>19</v>
       </c>
       <c r="B37">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C37">
         <v>5</v>
@@ -1414,11 +1414,11 @@
       </c>
       <c r="F37">
         <f t="shared" si="14"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G37" s="1">
         <f>(D37-B37+E37)*2</f>
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1642,7 +1642,7 @@
         <v>50</v>
       </c>
       <c r="G46">
-        <f t="shared" ref="G46:G47" si="17">D46-B46+E46</f>
+        <f t="shared" ref="G46" si="17">D46-B46+E46</f>
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change standing right punch animation and adjust move balance
</commit_message>
<xml_diff>
--- a/frameData.xlsx
+++ b/frameData.xlsx
@@ -452,7 +452,7 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -529,7 +529,7 @@
       </c>
       <c r="C4">
         <f t="shared" ref="C4:C18" si="2">F4+B4-E4+5</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D18" si="3">G4+B4-E4</f>
@@ -541,7 +541,7 @@
       </c>
       <c r="F4">
         <f t="shared" ref="F4:G23" si="5">F28</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G4">
         <f t="shared" si="5"/>
@@ -1179,7 +1179,7 @@
         <v>13</v>
       </c>
       <c r="C28">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D28">
         <v>-4</v>
@@ -1189,7 +1189,7 @@
       </c>
       <c r="F28">
         <f t="shared" ref="F28:F45" si="14">C28-B28+E28-5</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G28">
         <f>D28-B28+E28</f>
@@ -1242,7 +1242,7 @@
         <v>35</v>
       </c>
       <c r="G30">
-        <f t="shared" ref="G29:G45" si="15">D30-B30+E30</f>
+        <f t="shared" ref="G30:G45" si="15">D30-B30+E30</f>
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Build, correct minor mistakes
</commit_message>
<xml_diff>
--- a/frameData.xlsx
+++ b/frameData.xlsx
@@ -452,7 +452,7 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -529,7 +529,7 @@
       </c>
       <c r="C4">
         <f t="shared" ref="C4:C18" si="2">F4+B4-E4+5</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D18" si="3">G4+B4-E4</f>
@@ -541,7 +541,7 @@
       </c>
       <c r="F4">
         <f t="shared" ref="F4:G23" si="5">F28</f>
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G4">
         <f t="shared" si="5"/>
@@ -1179,7 +1179,7 @@
         <v>13</v>
       </c>
       <c r="C28">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D28">
         <v>-4</v>
@@ -1189,7 +1189,7 @@
       </c>
       <c r="F28">
         <f t="shared" ref="F28:F45" si="14">C28-B28+E28-5</f>
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G28">
         <f>D28-B28+E28</f>

</xml_diff>